<commit_message>
edit 21-30 and add new.md
</commit_message>
<xml_diff>
--- a/21-30.xlsx
+++ b/21-30.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aparna\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aparna\Documents\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5C9F73-A3E6-402C-9686-9F44AC593564}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAF5906-0E4D-4FD8-B04C-4F6358DAD12D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{C4994230-FB4E-494D-AB04-82F7ABC0C9B8}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="16200" windowHeight="10060" xr2:uid="{C4994230-FB4E-494D-AB04-82F7ABC0C9B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>s.no</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>sambusandeep20@gmail.com</t>
+  </si>
+  <si>
+    <t>i79x1a05b5</t>
   </si>
 </sst>
 </file>
@@ -495,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F3D0C1-352A-4DE8-B988-AADF0AB8D758}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -655,6 +658,11 @@
       </c>
       <c r="F11" s="1" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>